<commit_message>
Some final degree function changes
</commit_message>
<xml_diff>
--- a/Registrazioni-Voti.xlsx
+++ b/Registrazioni-Voti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cripp\Google Drive\programming\repos\pomodoro-email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CA2FD6-4445-44C1-9070-C8E670181188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F53582-6072-4DD2-85A9-3C7852B8B7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
   <si>
     <t>Analisi I</t>
   </si>
@@ -219,9 +219,6 @@
     <t>CFU</t>
   </si>
   <si>
-    <t>Progetto</t>
-  </si>
-  <si>
     <t>Progetto di Reti Logiche</t>
   </si>
   <si>
@@ -232,22 +229,32 @@
   </si>
   <si>
     <t>Progetto di Algoritmi e Principi dell'Informatica</t>
+  </si>
+  <si>
+    <t>Calcolo Numerico</t>
+  </si>
+  <si>
+    <t>Dedé</t>
+  </si>
+  <si>
+    <t>Fondamenti di Ricerca Operativa</t>
+  </si>
+  <si>
+    <t>Malucelli</t>
+  </si>
+  <si>
+    <t>EFFETTIVO</t>
+  </si>
+  <si>
+    <t>Prova Finale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -332,9 +339,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -617,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,15 +632,16 @@
     <col min="1" max="1" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="6"/>
     <col min="3" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -661,11 +666,14 @@
       <c r="H1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,11 +698,14 @@
       <c r="H2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -719,11 +730,14 @@
       <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -748,11 +762,14 @@
       <c r="H4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -777,11 +794,14 @@
       <c r="H5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,11 +826,14 @@
       <c r="H6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -835,11 +858,14 @@
       <c r="H7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -864,11 +890,14 @@
       <c r="H8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -893,11 +922,14 @@
       <c r="H9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -922,11 +954,14 @@
       <c r="H10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -951,11 +986,14 @@
       <c r="H11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -980,11 +1018,14 @@
       <c r="H12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1009,11 +1050,14 @@
       <c r="H13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1038,11 +1082,14 @@
       <c r="H14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1067,11 +1114,14 @@
       <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1096,11 +1146,14 @@
       <c r="H16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1125,11 +1178,14 @@
       <c r="H17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1154,11 +1210,14 @@
       <c r="H18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1183,16 +1242,19 @@
       <c r="H19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="6">
-        <v>1</v>
+      <c r="B20" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C20" s="6">
         <v>5</v>
@@ -1212,16 +1274,19 @@
       <c r="H20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C21" s="6">
         <v>5</v>
@@ -1241,16 +1306,19 @@
       <c r="H21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C22" s="6">
         <v>5</v>
@@ -1270,16 +1338,19 @@
       <c r="H22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="6">
-        <v>1</v>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="6">
         <v>8</v>
@@ -1297,96 +1368,172 @@
         <v>41</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>61</v>
+      <c r="B24" s="6">
+        <v>21</v>
       </c>
       <c r="C24" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B25" s="6">
         <v>1</v>
       </c>
-      <c r="C25" s="7">
-        <v>1</v>
+      <c r="C25" s="6">
+        <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="6">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="2">
+        <v>66</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="6">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>